<commit_message>
Update Relatorio-individual - Tiago.xlsx
</commit_message>
<xml_diff>
--- a/relatorios/Relatorio-individual - Tiago.xlsx
+++ b/relatorios/Relatorio-individual - Tiago.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marco/Library/CloudStorage/Dropbox/ESTG/_Aulas/2022-2023/2022-23-EI-AI/03.Projeto/Relatorio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigor\OneDrive\Desktop\EI\ainet\projetoAInet\relatorios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654B5FC7-2B8E-1E4F-BF03-30CE9ACF51F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7E81EC-FA2B-4910-93CE-03711BD01DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="BDut9OBXirJHuaqMATYSYY0IcZ39UhQaxY4ivSAxhWFjLbwvdCvaNwz18ggAeakjbAy9PwMeCa+bzZHwGDmDUQ==" workbookSaltValue="6WTzD8wUpr5dqEHlS3NsMw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rel. Individual Prj AI 2022-23" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
   <si>
     <t>Nº Grupo</t>
   </si>
@@ -407,13 +407,28 @@
       </rPr>
       <t xml:space="preserve"> relativos à avaliação dos colegas. </t>
     </r>
+  </si>
+  <si>
+    <t>Tiago José Figueira Pires Rodrigues dos Reis</t>
+  </si>
+  <si>
+    <t>Daniel Marques Gonçalves</t>
+  </si>
+  <si>
+    <t>João Pedro Da Rocha Valverde Martins</t>
+  </si>
+  <si>
+    <t>Completo</t>
+  </si>
+  <si>
+    <t>Parcial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -713,6 +728,31 @@
       <alignment horizontal="right" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
       <protection locked="0"/>
@@ -725,101 +765,20 @@
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -1105,34 +1064,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DEBAC6A-54C1-F842-B37B-99052CD80123}">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="22.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.296875" style="2" customWidth="1"/>
     <col min="3" max="3" width="4" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="2.1640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="6.1640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" style="2" customWidth="1"/>
-    <col min="10" max="12" width="27.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.69921875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="2.19921875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="6.19921875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.796875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="19.69921875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="19.796875" style="2" customWidth="1"/>
+    <col min="10" max="12" width="27.296875" style="2" customWidth="1"/>
     <col min="13" max="13" width="6.5" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="2"/>
+    <col min="14" max="16384" width="10.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="7" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="7.05" customHeight="1"/>
+    <row r="2" spans="1:13" ht="22.05" customHeight="1">
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1">
+        <v>10</v>
+      </c>
       <c r="F2" s="17" t="s">
         <v>6</v>
       </c>
@@ -1141,24 +1102,28 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="6" customHeight="1">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="22.05" customHeight="1">
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="33"/>
+      <c r="D4" s="33">
+        <v>2201793</v>
+      </c>
       <c r="E4" s="13"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="43"/>
-      <c r="H4" s="44"/>
+      <c r="G4" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="36"/>
       <c r="I4" s="13"/>
       <c r="J4" s="21" t="s">
         <v>14</v>
@@ -1167,7 +1132,7 @@
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
     </row>
-    <row r="5" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="22.05" customHeight="1">
       <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
@@ -1176,20 +1141,20 @@
       <c r="I5" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="22" t="str">
+      <c r="J5" s="22">
         <f>IF(D4&lt;&gt;"",D4,"")</f>
-        <v/>
-      </c>
-      <c r="K5" s="24" t="str">
+        <v>2201793</v>
+      </c>
+      <c r="K5" s="24">
         <f>IF(D6&lt;&gt;"",D6,"")</f>
-        <v/>
-      </c>
-      <c r="L5" s="24" t="str">
+        <v>2201790</v>
+      </c>
+      <c r="L5" s="24">
         <f>IF(D7&lt;&gt;"",D7,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+        <v>2182185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="22.05" customHeight="1">
       <c r="A6" s="12"/>
       <c r="B6" s="12" t="s">
         <v>9</v>
@@ -1197,41 +1162,49 @@
       <c r="C6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="11"/>
+      <c r="D6" s="11">
+        <v>2201790</v>
+      </c>
       <c r="F6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="45"/>
-      <c r="H6" s="46"/>
+      <c r="G6" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="38"/>
       <c r="I6" s="18" t="s">
         <v>2</v>
       </c>
       <c r="J6" s="22" t="str">
         <f>IF(G4&lt;&gt;"",G4,"")</f>
-        <v/>
+        <v>Tiago José Figueira Pires Rodrigues dos Reis</v>
       </c>
       <c r="K6" s="24" t="str">
         <f>IF(G6&lt;&gt;"",G6,"")</f>
-        <v/>
+        <v>Daniel Marques Gonçalves</v>
       </c>
       <c r="L6" s="24" t="str">
         <f>IF(G7&lt;&gt;"",G7,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+        <v>João Pedro Da Rocha Valverde Martins</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="22.05" customHeight="1">
       <c r="B7" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="11"/>
+      <c r="D7" s="11">
+        <v>2182185</v>
+      </c>
       <c r="F7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="45"/>
-      <c r="H7" s="46"/>
+      <c r="G7" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="38"/>
       <c r="I7" s="14"/>
       <c r="J7" s="22" t="s">
         <v>8</v>
@@ -1243,8 +1216,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:13" ht="8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="4.95" customHeight="1"/>
+    <row r="9" spans="1:13" ht="7.95" customHeight="1">
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
       <c r="D9" s="17"/>
@@ -1258,7 +1231,7 @@
       <c r="L9" s="17"/>
       <c r="M9" s="17"/>
     </row>
-    <row r="10" spans="1:13" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="28.95" customHeight="1">
       <c r="B10" s="26"/>
       <c r="C10" s="17" t="s">
         <v>18</v>
@@ -1273,127 +1246,127 @@
       <c r="L10" s="26"/>
       <c r="M10" s="26"/>
     </row>
-    <row r="11" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="39" customHeight="1">
       <c r="B11" s="14"/>
       <c r="C11" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="37"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
       <c r="M11" s="14"/>
     </row>
-    <row r="12" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="24" customHeight="1">
       <c r="B12" s="14"/>
       <c r="C12" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
       <c r="M12" s="14"/>
     </row>
-    <row r="13" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="24" customHeight="1">
       <c r="B13" s="14"/>
       <c r="C13" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="37"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
       <c r="M13" s="14"/>
     </row>
-    <row r="14" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="39" customHeight="1">
       <c r="B14" s="14"/>
       <c r="C14" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="37"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
       <c r="M14" s="14"/>
     </row>
-    <row r="15" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="39" customHeight="1">
       <c r="B15" s="14"/>
       <c r="C15" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
       <c r="M15" s="14"/>
     </row>
-    <row r="16" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="24" customHeight="1">
       <c r="B16" s="14"/>
       <c r="C16" s="27"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
       <c r="M16" s="14"/>
     </row>
-    <row r="17" spans="2:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:13" ht="27" customHeight="1">
       <c r="B17" s="14"/>
       <c r="C17" s="18"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="42" t="s">
+      <c r="F17" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
       <c r="M17" s="14"/>
     </row>
-    <row r="18" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" ht="18" customHeight="1">
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="28"/>
@@ -1401,17 +1374,17 @@
       <c r="F18" s="29">
         <v>0</v>
       </c>
-      <c r="G18" s="38" t="s">
+      <c r="G18" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
       <c r="J18" s="14"/>
       <c r="K18" s="14"/>
       <c r="L18" s="14"/>
       <c r="M18" s="14"/>
     </row>
-    <row r="19" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" ht="18" customHeight="1">
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="30"/>
@@ -1419,17 +1392,17 @@
       <c r="F19" s="29">
         <v>1</v>
       </c>
-      <c r="G19" s="38" t="s">
+      <c r="G19" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
       <c r="J19" s="14"/>
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
       <c r="M19" s="14"/>
     </row>
-    <row r="20" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" ht="18" customHeight="1">
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="30"/>
@@ -1437,17 +1410,17 @@
       <c r="F20" s="29">
         <v>2</v>
       </c>
-      <c r="G20" s="38" t="s">
+      <c r="G20" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
       <c r="J20" s="14"/>
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
       <c r="M20" s="14"/>
     </row>
-    <row r="21" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13" ht="18" customHeight="1">
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
@@ -1455,56 +1428,56 @@
       <c r="F21" s="29">
         <v>3</v>
       </c>
-      <c r="G21" s="38" t="s">
+      <c r="G21" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
       <c r="J21" s="14"/>
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
       <c r="M21" s="14"/>
     </row>
-    <row r="22" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13" ht="18" customHeight="1">
       <c r="F22" s="29">
         <v>4</v>
       </c>
-      <c r="G22" s="38" t="s">
+      <c r="G22" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-    </row>
-    <row r="23" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+    </row>
+    <row r="23" spans="2:13" ht="18" customHeight="1">
       <c r="F23" s="25">
         <v>5</v>
       </c>
-      <c r="G23" s="38" t="s">
+      <c r="G23" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-    </row>
-    <row r="24" spans="2:13" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+    </row>
+    <row r="24" spans="2:13" ht="10.050000000000001" customHeight="1">
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="2:13" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="40" t="s">
+    <row r="25" spans="2:13" ht="36" customHeight="1">
+      <c r="B25" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="45"/>
+      <c r="L25" s="45"/>
       <c r="M25" s="17"/>
     </row>
-    <row r="26" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:13" ht="28.95" customHeight="1">
       <c r="B26" s="8"/>
       <c r="C26" s="31"/>
       <c r="D26" s="31"/>
@@ -1515,12 +1488,18 @@
       </c>
       <c r="H26" s="39"/>
       <c r="I26" s="39"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
+      <c r="J26" s="23">
+        <v>1</v>
+      </c>
+      <c r="K26" s="20">
+        <v>4</v>
+      </c>
+      <c r="L26" s="20">
+        <v>3</v>
+      </c>
       <c r="M26" s="32"/>
     </row>
-    <row r="27" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:13" ht="28.95" customHeight="1">
       <c r="B27" s="8"/>
       <c r="C27" s="31"/>
       <c r="D27" s="31"/>
@@ -1531,12 +1510,18 @@
       </c>
       <c r="H27" s="39"/>
       <c r="I27" s="39"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
+      <c r="J27" s="23">
+        <v>3</v>
+      </c>
+      <c r="K27" s="20">
+        <v>4</v>
+      </c>
+      <c r="L27" s="20">
+        <v>4</v>
+      </c>
       <c r="M27" s="32"/>
     </row>
-    <row r="28" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:13" ht="28.95" customHeight="1">
       <c r="B28" s="8"/>
       <c r="C28" s="31"/>
       <c r="D28" s="31"/>
@@ -1547,29 +1532,35 @@
       </c>
       <c r="H28" s="39"/>
       <c r="I28" s="39"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
+      <c r="J28" s="23">
+        <v>2</v>
+      </c>
+      <c r="K28" s="20">
+        <v>2</v>
+      </c>
+      <c r="L28" s="20">
+        <v>1</v>
+      </c>
       <c r="M28" s="32"/>
     </row>
-    <row r="29" spans="2:13" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="2:13" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="41" t="s">
+    <row r="29" spans="2:13" ht="13.95" customHeight="1"/>
+    <row r="30" spans="2:13" ht="36" customHeight="1">
+      <c r="B30" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="41"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="46"/>
       <c r="M30" s="17"/>
     </row>
-    <row r="31" spans="2:13" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:13" ht="36" customHeight="1">
       <c r="B31" s="4">
         <v>1</v>
       </c>
@@ -1582,14 +1573,20 @@
       <c r="G31" s="39"/>
       <c r="H31" s="39"/>
       <c r="I31" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="J31" s="23"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
+        <v>47</v>
+      </c>
+      <c r="J31" s="23">
+        <v>2</v>
+      </c>
+      <c r="K31" s="20">
+        <v>4</v>
+      </c>
+      <c r="L31" s="20">
+        <v>4</v>
+      </c>
       <c r="M31" s="32"/>
     </row>
-    <row r="32" spans="2:13" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:13" ht="36" customHeight="1">
       <c r="B32" s="4">
         <v>2</v>
       </c>
@@ -1602,14 +1599,20 @@
       <c r="G32" s="39"/>
       <c r="H32" s="39"/>
       <c r="I32" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="J32" s="23">
+        <v>4</v>
+      </c>
+      <c r="K32" s="20">
         <v>3</v>
       </c>
-      <c r="J32" s="23"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
+      <c r="L32" s="20">
+        <v>2</v>
+      </c>
       <c r="M32" s="32"/>
     </row>
-    <row r="33" spans="2:13" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:13" ht="36" customHeight="1">
       <c r="B33" s="4">
         <v>3</v>
       </c>
@@ -1622,14 +1625,14 @@
       <c r="G33" s="39"/>
       <c r="H33" s="39"/>
       <c r="I33" s="15" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="J33" s="23"/>
       <c r="K33" s="20"/>
       <c r="L33" s="20"/>
       <c r="M33" s="32"/>
     </row>
-    <row r="34" spans="2:13" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:13" ht="36" customHeight="1">
       <c r="B34" s="4">
         <v>4</v>
       </c>
@@ -1649,7 +1652,7 @@
       <c r="L34" s="20"/>
       <c r="M34" s="32"/>
     </row>
-    <row r="35" spans="2:13" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:13" ht="36" customHeight="1">
       <c r="B35" s="4">
         <v>5</v>
       </c>
@@ -1662,14 +1665,14 @@
       <c r="G35" s="39"/>
       <c r="H35" s="39"/>
       <c r="I35" s="15" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="J35" s="23"/>
       <c r="K35" s="20"/>
       <c r="L35" s="20"/>
       <c r="M35" s="32"/>
     </row>
-    <row r="36" spans="2:13" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:13" ht="36" customHeight="1">
       <c r="B36" s="4">
         <v>6</v>
       </c>
@@ -1689,7 +1692,7 @@
       <c r="L36" s="20"/>
       <c r="M36" s="32"/>
     </row>
-    <row r="37" spans="2:13" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:13" ht="36" customHeight="1">
       <c r="B37" s="4">
         <v>7</v>
       </c>
@@ -1702,14 +1705,20 @@
       <c r="G37" s="39"/>
       <c r="H37" s="39"/>
       <c r="I37" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="J37" s="23"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="20"/>
+        <v>47</v>
+      </c>
+      <c r="J37" s="23">
+        <v>1</v>
+      </c>
+      <c r="K37" s="20">
+        <v>4</v>
+      </c>
+      <c r="L37" s="20">
+        <v>4</v>
+      </c>
       <c r="M37" s="32"/>
     </row>
-    <row r="38" spans="2:13" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:13" ht="36" customHeight="1">
       <c r="B38" s="4">
         <v>8</v>
       </c>
@@ -1729,48 +1738,48 @@
       <c r="L38" s="20"/>
       <c r="M38" s="32"/>
     </row>
-    <row r="39" spans="2:13" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="2:13" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="2:13" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="40" t="s">
+    <row r="39" spans="2:13" ht="13.95" customHeight="1"/>
+    <row r="40" spans="2:13" ht="13.95" customHeight="1"/>
+    <row r="41" spans="2:13" ht="36" customHeight="1">
+      <c r="B41" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="40"/>
-      <c r="D41" s="40"/>
-      <c r="E41" s="40"/>
-      <c r="F41" s="40"/>
-      <c r="G41" s="40"/>
-      <c r="H41" s="40"/>
-      <c r="I41" s="40"/>
-      <c r="J41" s="40"/>
-      <c r="K41" s="40"/>
-      <c r="L41" s="40"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="45"/>
+      <c r="J41" s="45"/>
+      <c r="K41" s="45"/>
+      <c r="L41" s="45"/>
       <c r="M41" s="17"/>
     </row>
-    <row r="42" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:13" ht="22.05" customHeight="1">
       <c r="B42" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
     </row>
-    <row r="43" spans="2:13" ht="130" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="34"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
-      <c r="K43" s="35"/>
-      <c r="L43" s="36"/>
+    <row r="43" spans="2:13" ht="130.05000000000001" customHeight="1">
+      <c r="B43" s="41"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
+      <c r="K43" s="42"/>
+      <c r="L43" s="43"/>
       <c r="M43" s="32"/>
     </row>
-    <row r="44" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="2:13" s="9" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:13" ht="15" customHeight="1"/>
+    <row r="45" spans="2:13" ht="15" customHeight="1"/>
+    <row r="46" spans="2:13" s="9" customFormat="1" ht="63" customHeight="1">
       <c r="B46" s="10" t="s">
         <v>5</v>
       </c>
@@ -1779,21 +1788,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="onmbOWdCnm5cP1tCBX124PYJkRYa7UjJ5Wx31CPS7y5Sorj7U6RUhIX/UZQKXEhv4LqPYYwe5jo/WvFi7Jl8ZQ==" saltValue="KLxTWiXr2tx1ZWQvXTTT1Q==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="31">
-    <mergeCell ref="D13:L13"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="D12:L12"/>
-    <mergeCell ref="C36:H36"/>
-    <mergeCell ref="C37:H37"/>
-    <mergeCell ref="C38:H38"/>
-    <mergeCell ref="D14:L14"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="C32:H32"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="C34:H34"/>
-    <mergeCell ref="F17:I17"/>
     <mergeCell ref="B43:L43"/>
     <mergeCell ref="D11:L11"/>
     <mergeCell ref="D16:L16"/>
@@ -1810,51 +1804,26 @@
     <mergeCell ref="B25:L25"/>
     <mergeCell ref="G26:I26"/>
     <mergeCell ref="C35:H35"/>
+    <mergeCell ref="C36:H36"/>
+    <mergeCell ref="C37:H37"/>
+    <mergeCell ref="C38:H38"/>
+    <mergeCell ref="D14:L14"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="C34:H34"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="D13:L13"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="D12:L12"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
-  <conditionalFormatting sqref="I31:L31 J37:L38">
-    <cfRule type="expression" dxfId="8" priority="44">
+  <conditionalFormatting sqref="I31:L38">
+    <cfRule type="expression" dxfId="0" priority="14">
       <formula>$I31="Não Implementado"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J32:L36">
-    <cfRule type="expression" dxfId="7" priority="42">
-      <formula>$I32="Não Implementado"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I33">
-    <cfRule type="expression" dxfId="6" priority="20">
-      <formula>$I33="Não Implementado"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I34">
-    <cfRule type="expression" dxfId="5" priority="18">
-      <formula>$I34="Não Implementado"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="expression" dxfId="4" priority="21">
-      <formula>$I32="Não Implementado"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I36">
-    <cfRule type="expression" dxfId="3" priority="16">
-      <formula>$I36="Não Implementado"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="expression" dxfId="2" priority="17">
-      <formula>$I35="Não Implementado"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
-    <cfRule type="expression" dxfId="1" priority="15">
-      <formula>$I37="Não Implementado"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I38">
-    <cfRule type="expression" dxfId="0" priority="14">
-      <formula>$I38="Não Implementado"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">

</xml_diff>